<commit_message>
Importing production excel ignoring "-" when searching well name
</commit_message>
<xml_diff>
--- a/server/test/data/production.xlsx
+++ b/server/test/data/production.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17224"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\OICE_16_974FA576_32C1D314_1CCC\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14355" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="SIGEP" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="67">
   <si>
     <t>ANP - Agência Nacional do Petroleo, Gás Natural e Biocombustíveis</t>
   </si>
@@ -168,18 +163,12 @@
     <t>PETROBRAS 08</t>
   </si>
   <si>
-    <t xml:space="preserve">7PM  0035DPRJS      </t>
-  </si>
-  <si>
     <t>PAMPO</t>
   </si>
   <si>
     <t>PLATAFORMA DE PAMPO-1</t>
   </si>
   <si>
-    <t xml:space="preserve">7AB  0060D RJS      </t>
-  </si>
-  <si>
     <t xml:space="preserve">7VM  0078DPRJS      </t>
   </si>
   <si>
@@ -220,17 +209,23 @@
   </si>
   <si>
     <t>PETROBRAS 48</t>
+  </si>
+  <si>
+    <t>7MRL0054RJS</t>
+  </si>
+  <si>
+    <t>7MRL0062DRJS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="###,###,##0.0000"/>
     <numFmt numFmtId="165" formatCode="###,###,##0.00000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,9 +343,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -388,9 +383,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -423,26 +418,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -475,26 +453,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -674,7 +635,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
@@ -697,7 +658,7 @@
     <col min="19" max="19" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -705,17 +666,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
@@ -768,7 +729,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="9" t="s">
@@ -799,7 +760,7 @@
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -858,7 +819,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -915,7 +876,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -972,7 +933,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -1031,7 +992,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -1090,7 +1051,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
@@ -1149,7 +1110,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1208,7 +1169,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -1216,13 +1177,11 @@
         <v>25</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>28</v>
@@ -1258,7 +1217,7 @@
         <v>462.57229999999998</v>
       </c>
       <c r="Q14" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R14" s="8" t="s">
         <v>31</v>
@@ -1267,18 +1226,16 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>52</v>
-      </c>
+      <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>36</v>
@@ -1326,7 +1283,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
@@ -1334,10 +1291,10 @@
         <v>25</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>42</v>
@@ -1385,7 +1342,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
@@ -1393,10 +1350,10 @@
         <v>25</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>27</v>
@@ -1444,7 +1401,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -1452,10 +1409,10 @@
         <v>25</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>27</v>
@@ -1503,7 +1460,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -1511,13 +1468,13 @@
         <v>25</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>28</v>
@@ -1553,7 +1510,7 @@
         <v>10996.1211</v>
       </c>
       <c r="Q19" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="R19" s="8" t="s">
         <v>31</v>
@@ -1562,7 +1519,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -1570,10 +1527,10 @@
         <v>25</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>27</v>
@@ -1612,7 +1569,7 @@
         <v>2361.4106000000002</v>
       </c>
       <c r="Q20" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R20" s="8" t="s">
         <v>31</v>
@@ -1621,7 +1578,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1629,13 +1586,13 @@
         <v>25</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>28</v>
@@ -1671,7 +1628,7 @@
         <v>333.98739999999998</v>
       </c>
       <c r="Q21" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="R21" s="8" t="s">
         <v>31</v>
@@ -1680,7 +1637,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -1688,10 +1645,10 @@
         <v>25</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>27</v>
@@ -1730,7 +1687,7 @@
         <v>2362.2296000000001</v>
       </c>
       <c r="Q22" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R22" s="8" t="s">
         <v>31</v>
@@ -1739,7 +1696,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>24</v>
       </c>
@@ -1747,13 +1704,13 @@
         <v>25</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>28</v>
@@ -1789,7 +1746,7 @@
         <v>6314.3090000000002</v>
       </c>
       <c r="Q23" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R23" s="8" t="s">
         <v>31</v>
@@ -1800,22 +1757,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:N5"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>

</xml_diff>